<commit_message>
Update Cloud Labs Login Credentials - Dynatrace - 18-22 Aug 2025 - BOA.xlsx
</commit_message>
<xml_diff>
--- a/Cloud Labs Login Credentials - Dynatrace - 18-22 Aug 2025 - BOA.xlsx
+++ b/Cloud Labs Login Credentials - Dynatrace - 18-22 Aug 2025 - BOA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VK_GIT\DT_BOA_18_08_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB010FB2-AC53-4632-8D03-7905AE182527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AD5027-55E8-4882-8EB3-025037852711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,9 +345,6 @@
     <t>100.24.4.226</t>
   </si>
   <si>
-    <t>44.203.54.111</t>
-  </si>
-  <si>
     <t>13.218.208.250</t>
   </si>
   <si>
@@ -403,6 +400,9 @@
   </si>
   <si>
     <t>USERNAME</t>
+  </si>
+  <si>
+    <t>35.173.232.119</t>
   </si>
 </sst>
 </file>
@@ -1051,6 +1051,7 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1081,7 +1082,6 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1529,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
@@ -1548,52 +1548,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
     </row>
     <row r="5" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
@@ -1614,11 +1614,11 @@
       <c r="F6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.45">
@@ -1641,7 +1641,7 @@
         <v>93</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>93</v>
@@ -1901,7 +1901,7 @@
         <v>93</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="I17" s="13" t="s">
         <v>93</v>
@@ -1927,7 +1927,7 @@
         <v>93</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I18" s="13" t="s">
         <v>93</v>
@@ -1953,7 +1953,7 @@
         <v>93</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>93</v>
@@ -1979,7 +1979,7 @@
         <v>93</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I20" s="13" t="s">
         <v>93</v>
@@ -2005,7 +2005,7 @@
         <v>93</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>93</v>
@@ -2031,7 +2031,7 @@
         <v>93</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I22" s="13" t="s">
         <v>93</v>
@@ -2057,7 +2057,7 @@
         <v>93</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I23" s="13" t="s">
         <v>93</v>
@@ -2083,7 +2083,7 @@
         <v>93</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I24" s="13" t="s">
         <v>93</v>
@@ -2109,7 +2109,7 @@
         <v>93</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I25" s="13" t="s">
         <v>93</v>
@@ -2135,7 +2135,7 @@
         <v>93</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I26" s="13" t="s">
         <v>93</v>
@@ -2161,7 +2161,7 @@
         <v>93</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I27" s="13" t="s">
         <v>93</v>
@@ -2187,7 +2187,7 @@
         <v>93</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>93</v>
@@ -2213,7 +2213,7 @@
         <v>93</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>93</v>
@@ -2239,7 +2239,7 @@
         <v>93</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>93</v>
@@ -2265,7 +2265,7 @@
         <v>93</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>93</v>
@@ -2291,7 +2291,7 @@
         <v>93</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I32" s="13" t="s">
         <v>93</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.45">
       <c r="H33" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>